<commit_message>
removed Peters 1994, Chen 2011 from RCF
</commit_message>
<xml_diff>
--- a/data/electrical_pulp_2024-09-30.xlsx
+++ b/data/electrical_pulp_2024-09-30.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrant/Documents/_projects01/_uic/_dentalPulp/_dental_ept/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1CA4DE-DBDD-714B-A8D6-E4D8D21AAFE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BE0F4E8-2840-5E4E-A668-2B537ECDDAA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="500" windowWidth="49400" windowHeight="28020" activeTab="2" xr2:uid="{417E1520-0CB9-EB4F-B0AC-2B8135F03933}"/>
+    <workbookView xWindow="980" yWindow="500" windowWidth="48640" windowHeight="25480" activeTab="3" xr2:uid="{417E1520-0CB9-EB4F-B0AC-2B8135F03933}"/>
   </bookViews>
   <sheets>
     <sheet name="histology" sheetId="1" r:id="rId1"/>
     <sheet name="histology total necrosis only" sheetId="6" r:id="rId2"/>
     <sheet name="clinical" sheetId="2" r:id="rId3"/>
     <sheet name="root_canal_filled" sheetId="4" r:id="rId4"/>
+    <sheet name="root_canal_filled_old" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="116">
   <si>
     <t xml:space="preserve">Bruno et al 2009 </t>
   </si>
@@ -366,6 +367,27 @@
   </si>
   <si>
     <t>Digilog</t>
+  </si>
+  <si>
+    <t>Assume non-root canal normal; no other reference</t>
+  </si>
+  <si>
+    <t>added</t>
+  </si>
+  <si>
+    <t>Paired with 8 patients contributing 2 pairs of teeth (not accounted for in analysis)</t>
+  </si>
+  <si>
+    <t>Up to 11 teeth tested per patient</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>ADD Sensitivity with subsequent</t>
+  </si>
+  <si>
+    <t>Exclude</t>
   </si>
 </sst>
 </file>
@@ -375,7 +397,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -394,8 +416,14 @@
       <name val="Aptos"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -404,13 +432,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39994506668294322"/>
-        <bgColor indexed="65"/>
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
       </patternFill>
     </fill>
   </fills>
@@ -425,10 +458,10 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -457,7 +490,20 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -776,10 +822,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BFD3F145-D3CA-5F4A-B12F-1F47DA6B7447}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1060,14 +1106,48 @@
         <v>37</v>
       </c>
     </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F11" s="3">
+        <f>SUM(F4:F7)</f>
+        <v>51</v>
+      </c>
+      <c r="G11" s="3">
+        <f>SUM(G4:G7)</f>
+        <v>43</v>
+      </c>
+      <c r="H11" s="3">
+        <f>SUM(H4:H7)</f>
+        <v>482</v>
+      </c>
+      <c r="I11" s="3">
+        <f>SUM(I4:I7)</f>
+        <v>20</v>
+      </c>
+    </row>
     <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>94</v>
       </c>
     </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F13" s="3">
+        <f>F11+G11</f>
+        <v>94</v>
+      </c>
+    </row>
     <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>95</v>
+      </c>
+      <c r="F14" s="3">
+        <f>H11+I11</f>
+        <v>502</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F15" s="3">
+        <f>F13/(F13+F14)</f>
+        <v>0.15771812080536912</v>
       </c>
     </row>
   </sheetData>
@@ -1350,10 +1430,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF7FD32-BDB5-2044-9BC3-16D5D91200CF}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1527,7 +1607,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="11" t="s">
         <v>34</v>
       </c>
       <c r="B5" t="s">
@@ -1734,7 +1814,7 @@
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="A11" s="11" t="s">
         <v>43</v>
       </c>
       <c r="B11" t="s">
@@ -1767,6 +1847,42 @@
       </c>
       <c r="M11" t="s">
         <v>107</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F12" s="5">
+        <f>SUM(F2:F11)</f>
+        <v>244</v>
+      </c>
+      <c r="G12" s="5">
+        <f>SUM(G2:G11)</f>
+        <v>87</v>
+      </c>
+      <c r="H12" s="5">
+        <f>SUM(H2:H11)</f>
+        <v>327</v>
+      </c>
+      <c r="I12" s="5">
+        <f>SUM(I2:I11)</f>
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F14" s="5">
+        <f>F12+G12</f>
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F15" s="5">
+        <f>H12+I12</f>
+        <v>370</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="F16" s="5">
+        <f>F14/(F14+F15)</f>
+        <v>0.47218259629101283</v>
       </c>
     </row>
   </sheetData>
@@ -1777,25 +1893,26 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B45A69F-C957-5D44-9C34-1EB25860C01A}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="25.83203125" style="6" customWidth="1"/>
+    <col min="1" max="1" width="38.83203125" style="6" customWidth="1"/>
     <col min="2" max="2" width="65.83203125" style="6" customWidth="1"/>
     <col min="3" max="3" width="30.83203125" style="6" customWidth="1"/>
-    <col min="4" max="4" width="50.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
     <col min="5" max="9" width="9.83203125" style="6" customWidth="1"/>
     <col min="10" max="10" width="15.83203125" style="6" customWidth="1"/>
     <col min="11" max="12" width="9.83203125" style="6" customWidth="1"/>
-    <col min="13" max="13" width="30.83203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="52.33203125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>21</v>
       </c>
@@ -1835,9 +1952,276 @@
       <c r="M1" s="6" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+      <c r="N1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="7">
+        <f>28/30</f>
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="F2" s="6">
+        <v>28</v>
+      </c>
+      <c r="G2" s="6">
+        <v>2</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L2" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="7">
+        <f t="shared" ref="E3:E7" si="0">F3/(F3+G3)</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="6">
+        <v>2</v>
+      </c>
+      <c r="G3" s="6">
+        <v>0</v>
+      </c>
+      <c r="M3" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F4" s="6">
+        <v>10</v>
+      </c>
+      <c r="G4" s="6">
+        <v>0</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A5" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E5" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9152542372881356</v>
+      </c>
+      <c r="F5" s="6">
+        <v>54</v>
+      </c>
+      <c r="G5" s="6">
+        <v>5</v>
+      </c>
+      <c r="H5" s="12">
+        <v>52</v>
+      </c>
+      <c r="I5" s="12">
+        <v>7</v>
+      </c>
+      <c r="K5" s="6">
+        <f>59*2</f>
+        <v>118</v>
+      </c>
+      <c r="L5" s="6">
+        <v>51</v>
+      </c>
+      <c r="M5" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N5" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="7">
+        <f t="shared" si="0"/>
+        <v>0.9</v>
+      </c>
+      <c r="F6" s="6">
+        <v>18</v>
+      </c>
+      <c r="G6" s="6">
+        <v>2</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="6">
+        <v>0</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="6">
+        <v>10</v>
+      </c>
+      <c r="G7" s="6">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" s="6">
+        <v>0</v>
+      </c>
+      <c r="K7" s="6">
+        <v>10</v>
+      </c>
+      <c r="M7" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H14" s="12"/>
+      <c r="I14" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CBF1CC1-0A54-1346-B75A-A57C96F055DF}">
+  <dimension ref="A1:N17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="38.83203125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="65.83203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="30.83203125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="6" customWidth="1"/>
+    <col min="5" max="9" width="9.83203125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="15.83203125" style="6" customWidth="1"/>
+    <col min="11" max="12" width="9.83203125" style="6" customWidth="1"/>
+    <col min="13" max="13" width="52.33203125" style="6" customWidth="1"/>
+    <col min="14" max="14" width="23.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K1" t="s">
+        <v>27</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
         <v>58</v>
       </c>
       <c r="B2" s="6" t="s">
@@ -1862,12 +2246,18 @@
       <c r="I2" s="6">
         <v>3</v>
       </c>
+      <c r="K2" s="6">
+        <v>121</v>
+      </c>
+      <c r="L2" s="6">
+        <v>20</v>
+      </c>
       <c r="M2" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A3" s="13" t="s">
         <v>71</v>
       </c>
       <c r="B3" s="6" t="s">
@@ -1886,11 +2276,20 @@
       <c r="G3" s="6">
         <v>2</v>
       </c>
+      <c r="K3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>113</v>
+      </c>
       <c r="M3" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N3" s="6" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
         <v>61</v>
       </c>
@@ -1901,7 +2300,7 @@
         <v>62</v>
       </c>
       <c r="E4" s="7">
-        <f t="shared" ref="E4:E9" si="0">F4/(F4+G4)</f>
+        <f t="shared" ref="E4:E10" si="0">F4/(F4+G4)</f>
         <v>1</v>
       </c>
       <c r="F4" s="6">
@@ -1913,8 +2312,11 @@
       <c r="M4" s="6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="N4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>63</v>
       </c>
@@ -1938,8 +2340,8 @@
         <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
         <v>65</v>
       </c>
       <c r="B6" s="6" t="s">
@@ -1958,8 +2360,27 @@
       <c r="G6" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="H6" s="12">
+        <v>52</v>
+      </c>
+      <c r="I6" s="12">
+        <v>7</v>
+      </c>
+      <c r="K6" s="6">
+        <f>59*2</f>
+        <v>118</v>
+      </c>
+      <c r="L6" s="6">
+        <v>51</v>
+      </c>
+      <c r="M6" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="N6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>67</v>
       </c>
@@ -1983,7 +2404,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>34</v>
       </c>
@@ -2013,7 +2434,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -2046,8 +2467,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A10" s="14" t="s">
         <v>67</v>
       </c>
       <c r="B10" s="6" t="s">
@@ -2057,7 +2478,7 @@
         <v>108</v>
       </c>
       <c r="E10" s="7">
-        <f t="shared" ref="E10" si="1">F10/(F10+G10)</f>
+        <f t="shared" si="0"/>
         <v>0.5901639344262295</v>
       </c>
       <c r="F10" s="10">
@@ -2068,6 +2489,12 @@
       </c>
       <c r="M10" s="6" t="s">
         <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="8:9" x14ac:dyDescent="0.2">
+      <c r="H17" s="12"/>
+      <c r="I17" s="6" t="s">
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add coupled forest plots
</commit_message>
<xml_diff>
--- a/data/electrical_pulp_2024-09-30.xlsx
+++ b/data/electrical_pulp_2024-09-30.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mgrant/Documents/_projects01/_uic/_dentalPulp/_dental_ept/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A13D1F3-FB8A-B344-8875-816E540E21E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D30968A-863F-EC46-9493-062DF6547923}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4880" yWindow="500" windowWidth="46320" windowHeight="25480" activeTab="4" xr2:uid="{417E1520-0CB9-EB4F-B0AC-2B8135F03933}"/>
+    <workbookView xWindow="4880" yWindow="500" windowWidth="46320" windowHeight="25480" activeTab="2" xr2:uid="{417E1520-0CB9-EB4F-B0AC-2B8135F03933}"/>
   </bookViews>
   <sheets>
     <sheet name="histology" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="clinical" sheetId="2" r:id="rId3"/>
     <sheet name="root_canal_filled" sheetId="4" r:id="rId4"/>
     <sheet name="root_canal_filled_old" sheetId="7" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="127">
   <si>
     <t xml:space="preserve">Bruno et al 2009 </t>
   </si>
@@ -388,6 +389,39 @@
   </si>
   <si>
     <t>Exclude</t>
+  </si>
+  <si>
+    <t>delete case study</t>
+  </si>
+  <si>
+    <t>+</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Vital</t>
+  </si>
+  <si>
+    <t>Nonvital</t>
+  </si>
+  <si>
+    <t>po</t>
+  </si>
+  <si>
+    <t>ept</t>
+  </si>
+  <si>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>cold</t>
+  </si>
+  <si>
+    <t>ref</t>
+  </si>
+  <si>
+    <t>TP</t>
   </si>
 </sst>
 </file>
@@ -825,7 +859,7 @@
   <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1161,7 +1195,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M8" activeCellId="1" sqref="A1 M8"/>
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1349,6 +1383,9 @@
       <c r="G6" s="4">
         <v>1</v>
       </c>
+      <c r="M6" s="2" t="s">
+        <v>116</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1432,8 +1469,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECF7FD32-BDB5-2044-9BC3-16D5D91200CF}">
   <dimension ref="A1:N16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1893,10 +1930,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B45A69F-C957-5D44-9C34-1EB25860C01A}">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1990,115 +2027,118 @@
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A3" s="6" t="s">
-        <v>61</v>
+      <c r="A3" s="13" t="s">
+        <v>63</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>74</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>62</v>
+        <v>32</v>
       </c>
       <c r="E3" s="7">
-        <f t="shared" ref="E3:E7" si="0">F3/(F3+G3)</f>
+        <f t="shared" ref="E3:E6" si="0">F3/(F3+G3)</f>
         <v>1</v>
       </c>
       <c r="F3" s="6">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="G3" s="6">
         <v>0</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="N3" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A4" s="6" t="s">
-        <v>63</v>
+      <c r="A4" s="13" t="s">
+        <v>65</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="E4" s="7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0.9152542372881356</v>
       </c>
       <c r="F4" s="6">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="G4" s="6">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="H4" s="12">
+        <v>52</v>
+      </c>
+      <c r="I4" s="12">
+        <v>7</v>
+      </c>
+      <c r="K4" s="6">
+        <f>59*2</f>
+        <v>118</v>
+      </c>
+      <c r="L4" s="6">
+        <v>51</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>64</v>
+        <v>109</v>
+      </c>
+      <c r="N4" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" s="13" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E5" s="7">
         <f t="shared" si="0"/>
-        <v>0.9152542372881356</v>
+        <v>0.9</v>
       </c>
       <c r="F5" s="6">
-        <v>54</v>
+        <v>18</v>
       </c>
       <c r="G5" s="6">
-        <v>5</v>
-      </c>
-      <c r="H5" s="12">
-        <v>52</v>
-      </c>
-      <c r="I5" s="12">
-        <v>7</v>
-      </c>
-      <c r="K5" s="6">
-        <f>59*2</f>
-        <v>118</v>
-      </c>
-      <c r="L5" s="6">
-        <v>51</v>
+        <v>2</v>
+      </c>
+      <c r="H5" s="6">
+        <v>0</v>
+      </c>
+      <c r="I5" s="6">
+        <v>0</v>
       </c>
       <c r="M5" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="N5" t="s">
-        <v>111</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>34</v>
+      <c r="A6" s="11" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>76</v>
+        <v>86</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E6" s="7">
+        <v>32</v>
+      </c>
+      <c r="E6" s="6">
         <f t="shared" si="0"/>
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F6" s="6">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="G6" s="6">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H6" s="6">
         <v>0</v>
@@ -2106,47 +2146,44 @@
       <c r="I6" s="6">
         <v>0</v>
       </c>
+      <c r="K6" s="6">
+        <v>10</v>
+      </c>
       <c r="M6" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="6">
-        <f t="shared" si="0"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H13" s="12"/>
+      <c r="I13" s="6" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E18" s="7">
+        <f>F18/(F18+G18)</f>
         <v>1</v>
       </c>
-      <c r="F7" s="6">
-        <v>10</v>
-      </c>
-      <c r="G7" s="6">
+      <c r="F18" s="6">
+        <v>2</v>
+      </c>
+      <c r="G18" s="6">
         <v>0</v>
       </c>
-      <c r="H7" s="6">
-        <v>0</v>
-      </c>
-      <c r="I7" s="6">
-        <v>0</v>
-      </c>
-      <c r="K7" s="6">
-        <v>10</v>
-      </c>
-      <c r="M7" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="H14" s="12"/>
-      <c r="I14" s="6" t="s">
-        <v>110</v>
+      <c r="M18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="N18" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -2159,7 +2196,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CBF1CC1-0A54-1346-B75A-A57C96F055DF}">
   <dimension ref="A1:N17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
@@ -2501,4 +2538,525 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0093773E-E153-6D4F-A03D-9AD2C4A094A4}">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>123</v>
+      </c>
+      <c r="E1" t="s">
+        <v>124</v>
+      </c>
+      <c r="F1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+      <c r="E2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E4" t="s">
+        <v>118</v>
+      </c>
+      <c r="F4" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E5" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>118</v>
+      </c>
+      <c r="C6" t="s">
+        <v>117</v>
+      </c>
+      <c r="D6" t="s">
+        <v>117</v>
+      </c>
+      <c r="E6" t="s">
+        <v>117</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s">
+        <v>117</v>
+      </c>
+      <c r="F7" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>117</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" t="s">
+        <v>118</v>
+      </c>
+      <c r="E8" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+      <c r="D9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E9" t="s">
+        <v>117</v>
+      </c>
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>117</v>
+      </c>
+      <c r="D10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E10" t="s">
+        <v>118</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" t="s">
+        <v>117</v>
+      </c>
+      <c r="D11" t="s">
+        <v>117</v>
+      </c>
+      <c r="E11" t="s">
+        <v>117</v>
+      </c>
+      <c r="F11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D12" t="s">
+        <v>117</v>
+      </c>
+      <c r="E12" t="s">
+        <v>118</v>
+      </c>
+      <c r="F12" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" t="s">
+        <v>118</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D14" t="s">
+        <v>118</v>
+      </c>
+      <c r="E14" t="s">
+        <v>118</v>
+      </c>
+      <c r="F14" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="D15" t="s">
+        <v>118</v>
+      </c>
+      <c r="E15" t="s">
+        <v>118</v>
+      </c>
+      <c r="F15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>117</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D16" t="s">
+        <v>118</v>
+      </c>
+      <c r="E16" t="s">
+        <v>117</v>
+      </c>
+      <c r="F16" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
+        <v>117</v>
+      </c>
+      <c r="D17" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" t="s">
+        <v>117</v>
+      </c>
+      <c r="F17" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>117</v>
+      </c>
+      <c r="C18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D18" t="s">
+        <v>117</v>
+      </c>
+      <c r="E18" t="s">
+        <v>117</v>
+      </c>
+      <c r="F18" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>117</v>
+      </c>
+      <c r="C19" t="s">
+        <v>117</v>
+      </c>
+      <c r="D19" t="s">
+        <v>118</v>
+      </c>
+      <c r="E19" t="s">
+        <v>118</v>
+      </c>
+      <c r="F19" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>117</v>
+      </c>
+      <c r="C20" t="s">
+        <v>117</v>
+      </c>
+      <c r="D20" t="s">
+        <v>117</v>
+      </c>
+      <c r="E20" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" t="s">
+        <v>117</v>
+      </c>
+      <c r="D21" t="s">
+        <v>118</v>
+      </c>
+      <c r="E21" t="s">
+        <v>118</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>118</v>
+      </c>
+      <c r="C22" t="s">
+        <v>117</v>
+      </c>
+      <c r="D22" t="s">
+        <v>117</v>
+      </c>
+      <c r="E22" t="s">
+        <v>117</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G23" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" t="s">
+        <v>118</v>
+      </c>
+      <c r="E24" t="s">
+        <v>118</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D25" t="s">
+        <v>117</v>
+      </c>
+      <c r="E25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F25" t="s">
+        <v>119</v>
+      </c>
+      <c r="I25">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>